<commit_message>
test cases 6 and 10
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data1.xlsx
+++ b/com.espn/src/test/resources/test_data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.espn/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1E27B5-ABB5-D94D-BEA5-1E24D11D9BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CF37C2-5C62-8844-A27B-9C3BBAB01FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" activeTab="6" xr2:uid="{7B928831-F53C-A542-9271-10D2139B6158}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" firstSheet="5" activeTab="9" xr2:uid="{7B928831-F53C-A542-9271-10D2139B6158}"/>
   </bookViews>
   <sheets>
     <sheet name="PacificTeams" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Golden State Warriors</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Brock Lesnar</t>
   </si>
   <si>
-    <t>2022-23 season stats</t>
-  </si>
-  <si>
     <t>Unfollow</t>
   </si>
   <si>
@@ -133,6 +130,12 @@
   </si>
   <si>
     <t>KOBE</t>
+  </si>
+  <si>
+    <t>Fight History</t>
+  </si>
+  <si>
+    <t>2022-23 SEASON STATS</t>
   </si>
 </sst>
 </file>
@@ -174,10 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +510,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -517,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -525,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -533,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -541,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -549,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -559,6 +563,105 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E754BA-4963-464F-815B-730EA1362BB7}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3E8765-E97E-BA43-9559-D33DE87114EE}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED7DEAE-0524-D643-B98B-5C40C4889FD5}">
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390D7303-5839-0441-8A7C-D68AFBE5CE6A}">
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -566,9 +669,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -580,18 +680,88 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3E8765-E97E-BA43-9559-D33DE87114EE}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562A714E-46DA-A445-A7D1-203BE3A34F7E}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.1640625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3CA0B6-B515-1B48-9718-97BB94EB8CB8}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D4BE5-E24C-CC4F-A21D-5F238BC81B5E}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E668148A-2E49-A04D-AD4F-6C6CFBA6D6BD}">
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="15.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -600,168 +770,6 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED7DEAE-0524-D643-B98B-5C40C4889FD5}">
-  <dimension ref="A2:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.1640625" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390D7303-5839-0441-8A7C-D68AFBE5CE6A}">
-  <dimension ref="A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562A714E-46DA-A445-A7D1-203BE3A34F7E}">
-  <dimension ref="A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.1640625" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3CA0B6-B515-1B48-9718-97BB94EB8CB8}">
-  <dimension ref="A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D4BE5-E24C-CC4F-A21D-5F238BC81B5E}">
-  <dimension ref="A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E668148A-2E49-A04D-AD4F-6C6CFBA6D6BD}">
-  <dimension ref="A2:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -822,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EDEC83-2F98-F840-BBBF-1642F619D8E5}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -836,7 +844,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +857,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:XFD1048576"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>